<commit_message>
Generalised recovery function representation. `recovery_95percentile` not required.
</commit_message>
<xml_diff>
--- a/tests/models/potable_water_treatment_plant/pwtp_400ML.xlsx
+++ b/tests/models/potable_water_treatment_plant/pwtp_400ML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/sifra/tests/models/potable_water_treatment_plant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{035298CD-8AD1-564D-A2B4-4B99FA41CD47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8524BB88-895E-114A-8041-369EC1435F23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16900" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="223">
   <si>
     <t>component_type</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1556,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1823,6 +1826,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6722,10 +6731,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B47" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G69" sqref="G2:G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -6734,20 +6743,20 @@
     <col min="2" max="2" width="28.5" style="5" customWidth="1"/>
     <col min="3" max="4" width="13.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" style="5" customWidth="1"/>
-    <col min="6" max="7" width="14.1640625" style="6" customWidth="1"/>
-    <col min="8" max="10" width="11.1640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="12" style="6" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="15.5" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="19.1640625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="65.6640625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="44.6640625" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="7"/>
+    <col min="6" max="8" width="14.1640625" style="94" customWidth="1"/>
+    <col min="9" max="11" width="11.1640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12" style="6" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="6" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="65.6640625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="44.6640625" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="26" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>213</v>
       </c>
@@ -6763,44 +6772,47 @@
       <c r="E1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="93" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="93" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="N1" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="O1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="P1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="Q1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="2" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A2" s="91">
         <v>1</v>
       </c>
@@ -6820,41 +6832,44 @@
         <v>0.8</v>
       </c>
       <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0.2</v>
       </c>
-      <c r="I2" s="45">
+      <c r="J2" s="45">
         <v>0.95</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M2" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N2" s="12">
+      <c r="O2" s="12">
         <v>0.2</v>
       </c>
-      <c r="O2" s="13">
-        <f t="shared" ref="O2:O41" si="0">P2/NORMINV(0.95,0,1)</f>
+      <c r="P2" s="13">
+        <f t="shared" ref="P2:P41" si="0">Q2/NORMINV(0.95,0,1)</f>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P2" s="14">
+      <c r="Q2" s="14">
         <v>0.1</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="3" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A3" s="91">
         <v>2</v>
       </c>
@@ -6874,41 +6889,44 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.8</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>0.7</v>
       </c>
-      <c r="I3" s="46">
+      <c r="J3" s="46">
         <v>0.75</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L3" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M3" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N3" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>0.5</v>
       </c>
-      <c r="O3" s="13">
+      <c r="P3" s="13">
         <f t="shared" si="0"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P3" s="14">
+      <c r="Q3" s="14">
         <v>0.1</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="R3" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="4" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A4" s="91">
         <v>3</v>
       </c>
@@ -6928,41 +6946,44 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G4" s="41">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="H4" s="41">
         <v>0.85</v>
       </c>
-      <c r="I4" s="46">
+      <c r="I4" s="41">
+        <v>0.85</v>
+      </c>
+      <c r="J4" s="46">
         <v>0.3</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K4" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M4" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N4" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N4" s="12">
-        <v>1</v>
-      </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
+        <v>1</v>
+      </c>
+      <c r="P4" s="13">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P4" s="14">
+      <c r="Q4" s="14">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="R4" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="5" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A5" s="91">
         <v>4</v>
       </c>
@@ -6982,41 +7003,44 @@
         <v>1.4</v>
       </c>
       <c r="G5" s="42">
+        <v>0</v>
+      </c>
+      <c r="H5" s="42">
         <v>0.8</v>
       </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="46">
+      <c r="I5" s="42">
+        <v>1</v>
+      </c>
+      <c r="J5" s="46">
         <v>0</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M5" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N5" s="12">
+      <c r="O5" s="12">
         <v>4.3</v>
       </c>
-      <c r="O5" s="13">
+      <c r="P5" s="13">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="14">
+        <v>1</v>
+      </c>
+      <c r="R5" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="6" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A6" s="91">
         <v>5</v>
       </c>
@@ -7036,41 +7060,44 @@
         <v>0.15</v>
       </c>
       <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
         <v>0.4</v>
       </c>
-      <c r="H6" s="43">
+      <c r="I6" s="43">
         <v>0.2</v>
       </c>
-      <c r="I6" s="45">
+      <c r="J6" s="45">
         <v>0.95</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M6" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N6" s="20">
+      <c r="O6" s="20">
         <v>3</v>
       </c>
-      <c r="O6" s="10">
+      <c r="P6" s="10">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P6" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="21">
+        <v>1</v>
+      </c>
+      <c r="R6" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="7" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A7" s="91">
         <v>6</v>
       </c>
@@ -7090,41 +7117,44 @@
         <v>0.3</v>
       </c>
       <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
         <v>0.4</v>
       </c>
-      <c r="H7" s="43">
+      <c r="I7" s="43">
         <v>0.4</v>
       </c>
-      <c r="I7" s="46">
+      <c r="J7" s="46">
         <v>0.75</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="K7" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L7" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M7" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N7" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N7" s="22">
+      <c r="O7" s="22">
         <v>20</v>
       </c>
-      <c r="O7" s="18">
+      <c r="P7" s="18">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P7" s="23">
+      <c r="Q7" s="23">
         <v>2</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="R7" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="8" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A8" s="91">
         <v>7</v>
       </c>
@@ -7144,41 +7174,44 @@
         <v>0.8</v>
       </c>
       <c r="G8" s="43">
+        <v>0</v>
+      </c>
+      <c r="H8" s="43">
         <v>0.4</v>
       </c>
-      <c r="H8" s="43">
+      <c r="I8" s="43">
         <v>0.75</v>
       </c>
-      <c r="I8" s="46">
+      <c r="J8" s="46">
         <v>0.3</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="K8" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L8" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M8" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N8" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N8" s="22">
+      <c r="O8" s="22">
         <v>60</v>
       </c>
-      <c r="O8" s="18">
+      <c r="P8" s="18">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P8" s="23">
+      <c r="Q8" s="23">
         <v>4</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="R8" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="9" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A9" s="91">
         <v>8</v>
       </c>
@@ -7198,42 +7231,45 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G9" s="43">
+        <v>0</v>
+      </c>
+      <c r="H9" s="43">
         <v>0.4</v>
       </c>
-      <c r="H9" s="43">
+      <c r="I9" s="43">
         <v>0.9</v>
       </c>
-      <c r="I9" s="46">
+      <c r="J9" s="46">
         <v>0</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="K9" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M9" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N9" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N9" s="24">
+      <c r="O9" s="24">
         <f>24*30/7</f>
         <v>102.85714285714286</v>
       </c>
-      <c r="O9" s="25">
+      <c r="P9" s="25">
         <f t="shared" si="0"/>
         <v>4.8636546552941553</v>
       </c>
-      <c r="P9" s="26">
+      <c r="Q9" s="26">
         <v>8</v>
       </c>
-      <c r="Q9" s="15" t="s">
+      <c r="R9" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="27" customFormat="1" ht="14" customHeight="1">
+    <row r="10" spans="1:18" s="27" customFormat="1" ht="14" customHeight="1">
       <c r="A10" s="91">
         <v>9</v>
       </c>
@@ -7253,41 +7289,44 @@
         <v>0.36</v>
       </c>
       <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.5</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0.2</v>
       </c>
-      <c r="I10" s="45">
+      <c r="J10" s="45">
         <v>0.95</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M10" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N10" s="12">
+      <c r="O10" s="12">
         <v>0.2</v>
       </c>
-      <c r="O10" s="13">
+      <c r="P10" s="13">
         <f t="shared" si="0"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P10" s="14">
+      <c r="Q10" s="14">
         <v>0.1</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="R10" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="11" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A11" s="91">
         <v>10</v>
       </c>
@@ -7307,41 +7346,44 @@
         <v>0.6</v>
       </c>
       <c r="G11" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
         <v>0.5</v>
       </c>
-      <c r="I11" s="46">
+      <c r="I11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="46">
         <v>0.75</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="K11" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L11" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M11" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N11" s="12">
+      <c r="O11" s="12">
         <v>0.5</v>
       </c>
-      <c r="O11" s="13">
+      <c r="P11" s="13">
         <f t="shared" si="0"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="P11" s="14">
+      <c r="Q11" s="14">
         <v>0.1</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="R11" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="12" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A12" s="91">
         <v>11</v>
       </c>
@@ -7361,41 +7403,44 @@
         <v>1.2</v>
       </c>
       <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
         <v>0.6</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>0.8</v>
       </c>
-      <c r="I12" s="46">
+      <c r="J12" s="46">
         <v>0.3</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="K12" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L12" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M12" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N12" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N12" s="12">
-        <v>1</v>
-      </c>
-      <c r="O12" s="13">
+      <c r="O12" s="12">
+        <v>1</v>
+      </c>
+      <c r="P12" s="13">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P12" s="14">
+      <c r="Q12" s="14">
         <v>0.5</v>
       </c>
-      <c r="Q12" s="15" t="s">
+      <c r="R12" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="13" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A13" s="91">
         <v>12</v>
       </c>
@@ -7415,41 +7460,44 @@
         <v>1.5</v>
       </c>
       <c r="G13" s="42">
+        <v>0</v>
+      </c>
+      <c r="H13" s="42">
         <v>0.6</v>
       </c>
-      <c r="H13" s="42">
-        <v>1</v>
-      </c>
-      <c r="I13" s="46">
+      <c r="I13" s="42">
+        <v>1</v>
+      </c>
+      <c r="J13" s="46">
         <v>0</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="K13" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L13" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M13" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N13" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N13" s="12">
+      <c r="O13" s="12">
         <v>4.3</v>
       </c>
-      <c r="O13" s="13">
+      <c r="P13" s="13">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P13" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="15" t="s">
+      <c r="Q13" s="14">
+        <v>1</v>
+      </c>
+      <c r="R13" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="14" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A14" s="91">
         <v>13</v>
       </c>
@@ -7469,41 +7517,44 @@
         <v>0.65</v>
       </c>
       <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.6</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>0.15</v>
       </c>
-      <c r="I14" s="45">
+      <c r="J14" s="45">
         <v>0.95</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M14" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N14" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N14" s="20">
-        <v>1</v>
-      </c>
-      <c r="O14" s="10">
+      <c r="O14" s="20">
+        <v>1</v>
+      </c>
+      <c r="P14" s="10">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P14" s="21">
+      <c r="Q14" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q14" s="15" t="s">
+      <c r="R14" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="15" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A15" s="91">
         <v>14</v>
       </c>
@@ -7523,41 +7574,44 @@
         <v>1</v>
       </c>
       <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.7</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>0.5</v>
       </c>
-      <c r="I15" s="46">
+      <c r="J15" s="46">
         <v>0.75</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="K15" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L15" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M15" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N15" s="22">
+      <c r="O15" s="22">
         <v>3</v>
       </c>
-      <c r="O15" s="18">
+      <c r="P15" s="18">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P15" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="15" t="s">
+      <c r="Q15" s="23">
+        <v>1</v>
+      </c>
+      <c r="R15" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="16" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A16" s="91">
         <v>15</v>
       </c>
@@ -7577,41 +7631,44 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G16" s="41">
+        <v>0</v>
+      </c>
+      <c r="H16" s="41">
         <v>0.6</v>
       </c>
-      <c r="H16" s="41">
+      <c r="I16" s="41">
         <v>0.8</v>
       </c>
-      <c r="I16" s="46">
+      <c r="J16" s="46">
         <v>0.3</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="K16" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M16" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N16" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N16" s="22">
+      <c r="O16" s="22">
         <v>15</v>
       </c>
-      <c r="O16" s="18">
+      <c r="P16" s="18">
         <f t="shared" si="0"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P16" s="23">
+      <c r="Q16" s="23">
         <v>3</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="R16" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="17" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A17" s="91">
         <v>16</v>
       </c>
@@ -7631,41 +7688,44 @@
         <v>1.3</v>
       </c>
       <c r="G17" s="42">
+        <v>0</v>
+      </c>
+      <c r="H17" s="42">
         <v>0.6</v>
       </c>
-      <c r="H17" s="42">
+      <c r="I17" s="42">
         <v>0.97</v>
       </c>
-      <c r="I17" s="46">
+      <c r="J17" s="46">
         <v>0</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="K17" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M17" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N17" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N17" s="22">
+      <c r="O17" s="22">
         <v>30</v>
       </c>
-      <c r="O17" s="18">
+      <c r="P17" s="18">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P17" s="23">
+      <c r="Q17" s="23">
         <v>4</v>
       </c>
-      <c r="Q17" s="15" t="s">
+      <c r="R17" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="18" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="91">
         <v>17</v>
       </c>
@@ -7685,41 +7745,44 @@
         <v>0.32</v>
       </c>
       <c r="G18" s="44">
+        <v>0</v>
+      </c>
+      <c r="H18" s="44">
         <v>0.6</v>
       </c>
-      <c r="H18" s="43">
+      <c r="I18" s="43">
         <v>0.2</v>
       </c>
-      <c r="I18" s="45">
+      <c r="J18" s="45">
         <v>0.95</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M18" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N18" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N18" s="20">
+      <c r="O18" s="20">
         <v>5</v>
       </c>
-      <c r="O18" s="10">
+      <c r="P18" s="10">
         <f t="shared" si="0"/>
         <v>0.1823870495735308</v>
       </c>
-      <c r="P18" s="21">
+      <c r="Q18" s="21">
         <v>0.3</v>
       </c>
-      <c r="Q18" s="15" t="s">
+      <c r="R18" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="19" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A19" s="91">
         <v>18</v>
       </c>
@@ -7739,41 +7802,44 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="G19" s="41">
+        <v>0</v>
+      </c>
+      <c r="H19" s="41">
         <v>0.6</v>
       </c>
-      <c r="H19" s="43">
+      <c r="I19" s="43">
         <v>0.5</v>
       </c>
-      <c r="I19" s="46">
+      <c r="J19" s="46">
         <v>0.75</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="K19" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L19" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M19" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N19" s="22">
+      <c r="O19" s="22">
         <v>10</v>
       </c>
-      <c r="O19" s="18">
+      <c r="P19" s="18">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P19" s="23">
+      <c r="Q19" s="23">
         <v>2</v>
       </c>
-      <c r="Q19" s="15" t="s">
+      <c r="R19" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="20" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A20" s="91">
         <v>19</v>
       </c>
@@ -7793,41 +7859,44 @@
         <v>1</v>
       </c>
       <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
         <v>0.6</v>
       </c>
-      <c r="H20" s="43">
+      <c r="I20" s="43">
         <v>0.8</v>
       </c>
-      <c r="I20" s="46">
+      <c r="J20" s="46">
         <v>0.3</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="K20" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L20" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M20" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N20" s="22">
+      <c r="O20" s="22">
         <v>21</v>
       </c>
-      <c r="O20" s="18">
+      <c r="P20" s="18">
         <f t="shared" si="0"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P20" s="23">
+      <c r="Q20" s="23">
         <v>3</v>
       </c>
-      <c r="Q20" s="15" t="s">
+      <c r="R20" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="21" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A21" s="91">
         <v>20</v>
       </c>
@@ -7847,42 +7916,45 @@
         <v>1.35</v>
       </c>
       <c r="G21" s="42">
+        <v>0</v>
+      </c>
+      <c r="H21" s="42">
         <v>0.6</v>
       </c>
-      <c r="H21" s="43">
+      <c r="I21" s="43">
         <v>0.95</v>
       </c>
-      <c r="I21" s="46">
+      <c r="J21" s="46">
         <v>0</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="K21" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L21" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M21" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N21" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N21" s="22">
+      <c r="O21" s="22">
         <f>10*30/7</f>
         <v>42.857142857142854</v>
       </c>
-      <c r="O21" s="18">
+      <c r="P21" s="18">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P21" s="23">
+      <c r="Q21" s="23">
         <v>4</v>
       </c>
-      <c r="Q21" s="15" t="s">
+      <c r="R21" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="22" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A22" s="91">
         <v>21</v>
       </c>
@@ -7902,41 +7974,44 @@
         <v>0.4</v>
       </c>
       <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.6</v>
       </c>
-      <c r="H22" s="44">
+      <c r="I22" s="44">
         <v>0.2</v>
       </c>
-      <c r="I22" s="45">
+      <c r="J22" s="45">
         <v>0.95</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M22" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N22" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N22" s="20">
+      <c r="O22" s="20">
         <v>5</v>
       </c>
-      <c r="O22" s="10">
+      <c r="P22" s="10">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P22" s="21">
+      <c r="Q22" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q22" s="15" t="s">
+      <c r="R22" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="23" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A23" s="91">
         <v>22</v>
       </c>
@@ -7956,41 +8031,44 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G23" s="41">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41">
         <v>0.6</v>
       </c>
-      <c r="H23" s="41">
+      <c r="I23" s="41">
         <v>0.7</v>
       </c>
-      <c r="I23" s="46">
+      <c r="J23" s="46">
         <v>0.75</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="K23" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L23" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M23" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N23" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N23" s="22">
+      <c r="O23" s="22">
         <v>17</v>
       </c>
-      <c r="O23" s="18">
+      <c r="P23" s="18">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P23" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="15" t="s">
+      <c r="Q23" s="23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="24" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A24" s="91">
         <v>23</v>
       </c>
@@ -8010,41 +8088,44 @@
         <v>0.9</v>
       </c>
       <c r="G24" s="41">
+        <v>0</v>
+      </c>
+      <c r="H24" s="41">
         <v>0.6</v>
       </c>
-      <c r="H24" s="41">
+      <c r="I24" s="41">
         <v>0.8</v>
       </c>
-      <c r="I24" s="46">
+      <c r="J24" s="46">
         <v>0.3</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="K24" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L24" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M24" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N24" s="22">
+      <c r="O24" s="22">
         <v>37</v>
       </c>
-      <c r="O24" s="18">
+      <c r="P24" s="18">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P24" s="23">
+      <c r="Q24" s="23">
         <v>2</v>
       </c>
-      <c r="Q24" s="15" t="s">
+      <c r="R24" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="25" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A25" s="91">
         <v>24</v>
       </c>
@@ -8064,42 +8145,45 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G25" s="42">
+        <v>0</v>
+      </c>
+      <c r="H25" s="42">
         <v>0.6</v>
       </c>
-      <c r="H25" s="42">
+      <c r="I25" s="42">
         <v>0.95</v>
       </c>
-      <c r="I25" s="46">
+      <c r="J25" s="46">
         <v>0</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="K25" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L25" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M25" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N25" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N25" s="22">
+      <c r="O25" s="22">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O25" s="18">
+      <c r="P25" s="18">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P25" s="23">
+      <c r="Q25" s="23">
         <v>4</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="R25" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="26" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A26" s="91">
         <v>25</v>
       </c>
@@ -8119,41 +8203,44 @@
         <v>0.25</v>
       </c>
       <c r="G26" s="44">
+        <v>0</v>
+      </c>
+      <c r="H26" s="44">
         <v>0.6</v>
       </c>
-      <c r="H26" s="44">
+      <c r="I26" s="44">
         <v>0.2</v>
       </c>
-      <c r="I26" s="45">
+      <c r="J26" s="45">
         <v>0.95</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M26" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N26" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N26" s="20">
-        <v>1</v>
-      </c>
-      <c r="O26" s="10">
+      <c r="O26" s="20">
+        <v>1</v>
+      </c>
+      <c r="P26" s="10">
         <f t="shared" si="0"/>
         <v>0.12159136638235388</v>
       </c>
-      <c r="P26" s="21">
+      <c r="Q26" s="21">
         <v>0.2</v>
       </c>
-      <c r="Q26" s="15" t="s">
+      <c r="R26" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="27" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A27" s="91">
         <v>26</v>
       </c>
@@ -8173,41 +8260,44 @@
         <v>0.36</v>
       </c>
       <c r="G27" s="41">
+        <v>0</v>
+      </c>
+      <c r="H27" s="41">
         <v>0.6</v>
       </c>
-      <c r="H27" s="41">
+      <c r="I27" s="41">
         <v>0.5</v>
       </c>
-      <c r="I27" s="46">
+      <c r="J27" s="46">
         <v>0.75</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="K27" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L27" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M27" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N27" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N27" s="22">
+      <c r="O27" s="22">
         <v>4</v>
       </c>
-      <c r="O27" s="18">
+      <c r="P27" s="18">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P27" s="23">
+      <c r="Q27" s="23">
         <v>0.5</v>
       </c>
-      <c r="Q27" s="15" t="s">
+      <c r="R27" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="28" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A28" s="91">
         <v>27</v>
       </c>
@@ -8227,41 +8317,44 @@
         <v>0.53</v>
       </c>
       <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
         <v>0.6</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>0.65</v>
       </c>
-      <c r="I28" s="46">
+      <c r="J28" s="46">
         <v>0.3</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="K28" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L28" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M28" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N28" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N28" s="22">
+      <c r="O28" s="22">
         <v>8</v>
       </c>
-      <c r="O28" s="18">
+      <c r="P28" s="18">
         <f t="shared" si="0"/>
         <v>0.91193524786765412</v>
       </c>
-      <c r="P28" s="23">
+      <c r="Q28" s="23">
         <v>1.5</v>
       </c>
-      <c r="Q28" s="15" t="s">
+      <c r="R28" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="29" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A29" s="91">
         <v>28</v>
       </c>
@@ -8281,41 +8374,44 @@
         <v>1</v>
       </c>
       <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
         <v>0.6</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <v>0.9</v>
       </c>
-      <c r="I29" s="46">
+      <c r="J29" s="46">
         <v>0</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="K29" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L29" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M29" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N29" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N29" s="22">
+      <c r="O29" s="22">
         <v>12</v>
       </c>
-      <c r="O29" s="18">
+      <c r="P29" s="18">
         <f t="shared" si="0"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P29" s="23">
+      <c r="Q29" s="23">
         <v>3</v>
       </c>
-      <c r="Q29" s="15" t="s">
+      <c r="R29" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="30" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A30" s="91">
         <v>29</v>
       </c>
@@ -8335,41 +8431,44 @@
         <v>0.25</v>
       </c>
       <c r="G30" s="44">
+        <v>0</v>
+      </c>
+      <c r="H30" s="44">
         <v>0.6</v>
       </c>
-      <c r="H30" s="44">
+      <c r="I30" s="44">
         <v>0.2</v>
       </c>
-      <c r="I30" s="45">
+      <c r="J30" s="45">
         <v>0.95</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L30" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M30" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N30" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N30" s="20">
-        <v>1</v>
-      </c>
-      <c r="O30" s="10">
-        <f t="shared" ref="O30:O37" si="1">P30/NORMINV(0.95,0,1)</f>
+      <c r="O30" s="20">
+        <v>1</v>
+      </c>
+      <c r="P30" s="10">
+        <f t="shared" ref="P30:P37" si="1">Q30/NORMINV(0.95,0,1)</f>
         <v>0.12159136638235388</v>
       </c>
-      <c r="P30" s="21">
+      <c r="Q30" s="21">
         <v>0.2</v>
       </c>
-      <c r="Q30" s="15" t="s">
+      <c r="R30" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="31" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A31" s="91">
         <v>30</v>
       </c>
@@ -8389,41 +8488,44 @@
         <v>0.36</v>
       </c>
       <c r="G31" s="41">
+        <v>0</v>
+      </c>
+      <c r="H31" s="41">
         <v>0.6</v>
       </c>
-      <c r="H31" s="41">
+      <c r="I31" s="41">
         <v>0.5</v>
       </c>
-      <c r="I31" s="46">
+      <c r="J31" s="46">
         <v>0.75</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="K31" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L31" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M31" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N31" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N31" s="22">
+      <c r="O31" s="22">
         <v>4</v>
       </c>
-      <c r="O31" s="18">
+      <c r="P31" s="18">
         <f t="shared" si="1"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P31" s="23">
+      <c r="Q31" s="23">
         <v>0.5</v>
       </c>
-      <c r="Q31" s="15" t="s">
+      <c r="R31" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="32" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A32" s="91">
         <v>31</v>
       </c>
@@ -8443,41 +8545,44 @@
         <v>0.53</v>
       </c>
       <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
         <v>0.6</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>0.65</v>
       </c>
-      <c r="I32" s="46">
+      <c r="J32" s="46">
         <v>0.3</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="K32" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L32" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M32" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N32" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N32" s="22">
+      <c r="O32" s="22">
         <v>8</v>
       </c>
-      <c r="O32" s="18">
+      <c r="P32" s="18">
         <f t="shared" si="1"/>
         <v>0.91193524786765412</v>
       </c>
-      <c r="P32" s="23">
+      <c r="Q32" s="23">
         <v>1.5</v>
       </c>
-      <c r="Q32" s="15" t="s">
+      <c r="R32" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="33" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A33" s="91">
         <v>32</v>
       </c>
@@ -8497,41 +8602,44 @@
         <v>1</v>
       </c>
       <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
         <v>0.6</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>0.9</v>
       </c>
-      <c r="I33" s="46">
+      <c r="J33" s="46">
         <v>0</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="K33" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L33" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M33" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N33" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N33" s="22">
+      <c r="O33" s="22">
         <v>12</v>
       </c>
-      <c r="O33" s="18">
+      <c r="P33" s="18">
         <f t="shared" si="1"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P33" s="23">
+      <c r="Q33" s="23">
         <v>3</v>
       </c>
-      <c r="Q33" s="15" t="s">
+      <c r="R33" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="34" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A34" s="91">
         <v>33</v>
       </c>
@@ -8551,41 +8659,44 @@
         <v>0.25</v>
       </c>
       <c r="G34" s="44">
+        <v>0</v>
+      </c>
+      <c r="H34" s="44">
         <v>0.6</v>
       </c>
-      <c r="H34" s="44">
+      <c r="I34" s="44">
         <v>0.2</v>
       </c>
-      <c r="I34" s="45">
+      <c r="J34" s="45">
         <v>0.95</v>
       </c>
-      <c r="J34" s="11" t="s">
+      <c r="K34" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M34" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N34" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N34" s="20">
-        <v>1</v>
-      </c>
-      <c r="O34" s="10">
+      <c r="O34" s="20">
+        <v>1</v>
+      </c>
+      <c r="P34" s="10">
         <f t="shared" si="1"/>
         <v>0.12159136638235388</v>
       </c>
-      <c r="P34" s="21">
+      <c r="Q34" s="21">
         <v>0.2</v>
       </c>
-      <c r="Q34" s="15" t="s">
+      <c r="R34" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="35" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A35" s="91">
         <v>34</v>
       </c>
@@ -8605,41 +8716,44 @@
         <v>0.36</v>
       </c>
       <c r="G35" s="41">
+        <v>0</v>
+      </c>
+      <c r="H35" s="41">
         <v>0.6</v>
       </c>
-      <c r="H35" s="41">
+      <c r="I35" s="41">
         <v>0.5</v>
       </c>
-      <c r="I35" s="46">
+      <c r="J35" s="46">
         <v>0.75</v>
       </c>
-      <c r="J35" s="19" t="s">
+      <c r="K35" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L35" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M35" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N35" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N35" s="22">
+      <c r="O35" s="22">
         <v>4</v>
       </c>
-      <c r="O35" s="18">
+      <c r="P35" s="18">
         <f t="shared" si="1"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P35" s="23">
+      <c r="Q35" s="23">
         <v>0.5</v>
       </c>
-      <c r="Q35" s="15" t="s">
+      <c r="R35" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="36" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A36" s="91">
         <v>35</v>
       </c>
@@ -8659,41 +8773,44 @@
         <v>0.53</v>
       </c>
       <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
         <v>0.6</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>0.65</v>
       </c>
-      <c r="I36" s="46">
+      <c r="J36" s="46">
         <v>0.3</v>
       </c>
-      <c r="J36" s="19" t="s">
+      <c r="K36" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K36" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L36" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M36" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N36" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N36" s="22">
+      <c r="O36" s="22">
         <v>8</v>
       </c>
-      <c r="O36" s="18">
+      <c r="P36" s="18">
         <f t="shared" si="1"/>
         <v>0.91193524786765412</v>
       </c>
-      <c r="P36" s="23">
+      <c r="Q36" s="23">
         <v>1.5</v>
       </c>
-      <c r="Q36" s="15" t="s">
+      <c r="R36" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="37" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A37" s="91">
         <v>36</v>
       </c>
@@ -8713,41 +8830,44 @@
         <v>1</v>
       </c>
       <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
         <v>0.6</v>
       </c>
-      <c r="H37" s="3">
+      <c r="I37" s="3">
         <v>0.9</v>
       </c>
-      <c r="I37" s="46">
+      <c r="J37" s="46">
         <v>0</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="K37" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L37" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M37" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N37" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N37" s="22">
+      <c r="O37" s="22">
         <v>12</v>
       </c>
-      <c r="O37" s="18">
+      <c r="P37" s="18">
         <f t="shared" si="1"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="P37" s="23">
+      <c r="Q37" s="23">
         <v>3</v>
       </c>
-      <c r="Q37" s="15" t="s">
+      <c r="R37" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="38" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A38" s="91">
         <v>37</v>
       </c>
@@ -8767,41 +8887,44 @@
         <v>0.4</v>
       </c>
       <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
         <v>0.6</v>
       </c>
-      <c r="H38" s="44">
+      <c r="I38" s="44">
         <v>0.2</v>
       </c>
-      <c r="I38" s="45">
+      <c r="J38" s="45">
         <v>0.95</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="K38" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L38" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M38" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N38" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N38" s="20">
+      <c r="O38" s="20">
         <v>3</v>
       </c>
-      <c r="O38" s="10">
+      <c r="P38" s="10">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P38" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="15" t="s">
+      <c r="Q38" s="21">
+        <v>1</v>
+      </c>
+      <c r="R38" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="39" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A39" s="91">
         <v>38</v>
       </c>
@@ -8821,41 +8944,44 @@
         <v>0.67</v>
       </c>
       <c r="G39" s="41">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="H39" s="41">
         <v>0.7</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="41">
+        <v>0.7</v>
+      </c>
+      <c r="J39" s="46">
         <v>0.75</v>
       </c>
-      <c r="J39" s="19" t="s">
+      <c r="K39" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K39" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L39" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M39" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N39" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N39" s="22">
+      <c r="O39" s="22">
         <v>20</v>
       </c>
-      <c r="O39" s="18">
+      <c r="P39" s="18">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P39" s="23">
+      <c r="Q39" s="23">
         <v>2</v>
       </c>
-      <c r="Q39" s="15" t="s">
+      <c r="R39" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="40" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A40" s="91">
         <v>39</v>
       </c>
@@ -8875,41 +9001,44 @@
         <v>0.85</v>
       </c>
       <c r="G40" s="41">
+        <v>0</v>
+      </c>
+      <c r="H40" s="41">
         <v>0.7</v>
       </c>
-      <c r="H40" s="41">
+      <c r="I40" s="41">
         <v>0.85</v>
       </c>
-      <c r="I40" s="46">
+      <c r="J40" s="46">
         <v>0.3</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="K40" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K40" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L40" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M40" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N40" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N40" s="22">
+      <c r="O40" s="22">
         <v>60</v>
       </c>
-      <c r="O40" s="18">
+      <c r="P40" s="18">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P40" s="23">
+      <c r="Q40" s="23">
         <v>4</v>
       </c>
-      <c r="Q40" s="15" t="s">
+      <c r="R40" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="41" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A41" s="91">
         <v>40</v>
       </c>
@@ -8929,42 +9058,45 @@
         <v>1</v>
       </c>
       <c r="G41" s="42">
+        <v>0</v>
+      </c>
+      <c r="H41" s="42">
         <v>0.7</v>
       </c>
-      <c r="H41" s="42">
+      <c r="I41" s="42">
         <v>0.99</v>
       </c>
-      <c r="I41" s="46">
+      <c r="J41" s="46">
         <v>0</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="K41" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L41" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M41" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N41" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N41" s="22">
+      <c r="O41" s="22">
         <f>24*30/7</f>
         <v>102.85714285714286</v>
       </c>
-      <c r="O41" s="18">
+      <c r="P41" s="18">
         <f t="shared" si="0"/>
         <v>4.8636546552941553</v>
       </c>
-      <c r="P41" s="23">
+      <c r="Q41" s="23">
         <v>8</v>
       </c>
-      <c r="Q41" s="15" t="s">
+      <c r="R41" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="42" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A42" s="91">
         <v>41</v>
       </c>
@@ -8984,41 +9116,44 @@
         <v>0.4</v>
       </c>
       <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
         <v>0.7</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>0.2</v>
       </c>
-      <c r="I42" s="45">
+      <c r="J42" s="45">
         <v>0.95</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="K42" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K42" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M42" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N42" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N42" s="20">
+      <c r="O42" s="20">
         <v>5</v>
       </c>
-      <c r="O42" s="10">
-        <f t="shared" ref="O42:O61" si="2">P42/NORMINV(0.95,0,1)</f>
+      <c r="P42" s="10">
+        <f t="shared" ref="P42:P61" si="2">Q42/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P42" s="21">
+      <c r="Q42" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q42" s="15" t="s">
+      <c r="R42" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="43" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A43" s="91">
         <v>42</v>
       </c>
@@ -9038,41 +9173,44 @@
         <v>0.65</v>
       </c>
       <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
         <v>0.7</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>0.75</v>
       </c>
-      <c r="I43" s="46">
+      <c r="J43" s="46">
         <v>0.75</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="K43" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K43" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L43" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M43" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N43" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N43" s="22">
+      <c r="O43" s="22">
         <v>17</v>
       </c>
-      <c r="O43" s="18">
+      <c r="P43" s="18">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P43" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="15" t="s">
+      <c r="Q43" s="23">
+        <v>1</v>
+      </c>
+      <c r="R43" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="44" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A44" s="91">
         <v>43</v>
       </c>
@@ -9092,41 +9230,44 @@
         <v>0.95</v>
       </c>
       <c r="G44" s="41">
+        <v>0</v>
+      </c>
+      <c r="H44" s="41">
         <v>0.7</v>
       </c>
-      <c r="H44" s="41">
+      <c r="I44" s="41">
         <v>0.85</v>
       </c>
-      <c r="I44" s="46">
+      <c r="J44" s="46">
         <v>0.3</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="K44" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K44" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L44" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M44" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N44" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N44" s="22">
+      <c r="O44" s="22">
         <v>37</v>
       </c>
-      <c r="O44" s="18">
+      <c r="P44" s="18">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P44" s="23">
+      <c r="Q44" s="23">
         <v>2</v>
       </c>
-      <c r="Q44" s="15" t="s">
+      <c r="R44" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="45" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A45" s="91">
         <v>44</v>
       </c>
@@ -9146,42 +9287,45 @@
         <v>1.18</v>
       </c>
       <c r="G45" s="42">
+        <v>0</v>
+      </c>
+      <c r="H45" s="42">
         <v>0.7</v>
       </c>
-      <c r="H45" s="42">
+      <c r="I45" s="42">
         <v>0.9</v>
       </c>
-      <c r="I45" s="46">
+      <c r="J45" s="46">
         <v>0</v>
       </c>
-      <c r="J45" s="19" t="s">
+      <c r="K45" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K45" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M45" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N45" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N45" s="22">
+      <c r="O45" s="22">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O45" s="18">
+      <c r="P45" s="18">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P45" s="23">
+      <c r="Q45" s="23">
         <v>4</v>
       </c>
-      <c r="Q45" s="15" t="s">
+      <c r="R45" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="46" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A46" s="91">
         <v>45</v>
       </c>
@@ -9201,41 +9345,44 @@
         <v>0.25</v>
       </c>
       <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H46" s="44">
+      <c r="I46" s="44">
         <v>0.2</v>
       </c>
-      <c r="I46" s="45">
+      <c r="J46" s="45">
         <v>0.95</v>
       </c>
-      <c r="J46" s="11" t="s">
+      <c r="K46" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M46" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N46" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N46" s="20">
+      <c r="O46" s="20">
         <v>5</v>
       </c>
-      <c r="O46" s="10">
+      <c r="P46" s="10">
         <f t="shared" si="2"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P46" s="21">
+      <c r="Q46" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q46" s="15" t="s">
+      <c r="R46" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="47" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A47" s="91">
         <v>46</v>
       </c>
@@ -9255,41 +9402,44 @@
         <v>0.52</v>
       </c>
       <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
         <v>0.7</v>
       </c>
-      <c r="H47" s="41">
+      <c r="I47" s="41">
         <v>0.7</v>
       </c>
-      <c r="I47" s="46">
+      <c r="J47" s="46">
         <v>0.75</v>
       </c>
-      <c r="J47" s="19" t="s">
+      <c r="K47" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K47" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L47" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M47" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N47" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N47" s="22">
+      <c r="O47" s="22">
         <v>17</v>
       </c>
-      <c r="O47" s="18">
+      <c r="P47" s="18">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P47" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="15" t="s">
+      <c r="Q47" s="23">
+        <v>1</v>
+      </c>
+      <c r="R47" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="48" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A48" s="91">
         <v>47</v>
       </c>
@@ -9309,41 +9459,44 @@
         <v>0.95</v>
       </c>
       <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
         <v>0.6</v>
       </c>
-      <c r="H48" s="41">
+      <c r="I48" s="41">
         <v>0.8</v>
       </c>
-      <c r="I48" s="46">
+      <c r="J48" s="46">
         <v>0.3</v>
       </c>
-      <c r="J48" s="19" t="s">
+      <c r="K48" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K48" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M48" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N48" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N48" s="22">
+      <c r="O48" s="22">
         <v>37</v>
       </c>
-      <c r="O48" s="18">
+      <c r="P48" s="18">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P48" s="23">
+      <c r="Q48" s="23">
         <v>2</v>
       </c>
-      <c r="Q48" s="15" t="s">
+      <c r="R48" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="49" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A49" s="91">
         <v>48</v>
       </c>
@@ -9363,42 +9516,45 @@
         <v>1.64</v>
       </c>
       <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
         <v>0.7</v>
       </c>
-      <c r="H49" s="42">
+      <c r="I49" s="42">
         <v>0.99</v>
       </c>
-      <c r="I49" s="46">
+      <c r="J49" s="46">
         <v>0</v>
       </c>
-      <c r="J49" s="19" t="s">
+      <c r="K49" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K49" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L49" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M49" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N49" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N49" s="22">
+      <c r="O49" s="22">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O49" s="18">
+      <c r="P49" s="18">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P49" s="23">
+      <c r="Q49" s="23">
         <v>4</v>
       </c>
-      <c r="Q49" s="15" t="s">
+      <c r="R49" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="50" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A50" s="91">
         <v>49</v>
       </c>
@@ -9418,41 +9574,44 @@
         <v>0.53</v>
       </c>
       <c r="G50" s="44">
+        <v>0</v>
+      </c>
+      <c r="H50" s="44">
         <v>0.63</v>
       </c>
-      <c r="H50" s="44">
+      <c r="I50" s="44">
         <v>0.2</v>
       </c>
-      <c r="I50" s="45">
+      <c r="J50" s="45">
         <v>0.95</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="K50" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L50" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M50" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N50" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N50" s="20">
+      <c r="O50" s="20">
         <v>5</v>
       </c>
-      <c r="O50" s="10">
+      <c r="P50" s="10">
         <f t="shared" si="2"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P50" s="21">
+      <c r="Q50" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q50" s="15" t="s">
+      <c r="R50" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="51" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A51" s="91">
         <v>50</v>
       </c>
@@ -9472,41 +9631,44 @@
         <v>0.92</v>
       </c>
       <c r="G51" s="41">
+        <v>0</v>
+      </c>
+      <c r="H51" s="41">
         <v>0.65</v>
       </c>
-      <c r="H51" s="41">
+      <c r="I51" s="41">
         <v>0.45</v>
       </c>
-      <c r="I51" s="46">
+      <c r="J51" s="46">
         <v>0.75</v>
       </c>
-      <c r="J51" s="19" t="s">
+      <c r="K51" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L51" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M51" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N51" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N51" s="22">
+      <c r="O51" s="22">
         <v>17</v>
       </c>
-      <c r="O51" s="18">
+      <c r="P51" s="18">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P51" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="15" t="s">
+      <c r="Q51" s="23">
+        <v>1</v>
+      </c>
+      <c r="R51" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="52" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A52" s="91">
         <v>51</v>
       </c>
@@ -9526,41 +9688,44 @@
         <v>1.6</v>
       </c>
       <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
         <v>0.6</v>
       </c>
-      <c r="H52" s="2">
+      <c r="I52" s="2">
         <v>0.75</v>
       </c>
-      <c r="I52" s="46">
+      <c r="J52" s="46">
         <v>0.3</v>
       </c>
-      <c r="J52" s="19" t="s">
+      <c r="K52" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K52" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L52" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M52" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N52" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N52" s="22">
+      <c r="O52" s="22">
         <v>37</v>
       </c>
-      <c r="O52" s="18">
+      <c r="P52" s="18">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P52" s="23">
+      <c r="Q52" s="23">
         <v>2</v>
       </c>
-      <c r="Q52" s="15" t="s">
+      <c r="R52" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="53" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A53" s="91">
         <v>52</v>
       </c>
@@ -9580,42 +9745,45 @@
         <v>1.8</v>
       </c>
       <c r="G53" s="42">
+        <v>0</v>
+      </c>
+      <c r="H53" s="42">
         <v>0.6</v>
       </c>
-      <c r="H53" s="42">
+      <c r="I53" s="42">
         <v>0.95</v>
       </c>
-      <c r="I53" s="46">
+      <c r="J53" s="46">
         <v>0</v>
       </c>
-      <c r="J53" s="19" t="s">
+      <c r="K53" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K53" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L53" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M53" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N53" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N53" s="22">
+      <c r="O53" s="22">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O53" s="18">
+      <c r="P53" s="18">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P53" s="23">
+      <c r="Q53" s="23">
         <v>4</v>
       </c>
-      <c r="Q53" s="15" t="s">
+      <c r="R53" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="54" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A54" s="91">
         <v>53</v>
       </c>
@@ -9635,41 +9803,44 @@
         <v>0.6</v>
       </c>
       <c r="G54" s="44">
+        <v>0</v>
+      </c>
+      <c r="H54" s="44">
         <v>0.6</v>
       </c>
-      <c r="H54" s="44">
+      <c r="I54" s="44">
         <v>0.2</v>
       </c>
-      <c r="I54" s="45">
+      <c r="J54" s="45">
         <v>0.95</v>
       </c>
-      <c r="J54" s="11" t="s">
+      <c r="K54" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="K54" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="L54" s="11" t="s">
         <v>218</v>
       </c>
       <c r="M54" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N54" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="N54" s="20">
+      <c r="O54" s="20">
         <v>5</v>
       </c>
-      <c r="O54" s="10">
+      <c r="P54" s="10">
         <f t="shared" si="2"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="P54" s="21">
+      <c r="Q54" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q54" s="15" t="s">
+      <c r="R54" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="55" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A55" s="91">
         <v>54</v>
       </c>
@@ -9689,41 +9860,44 @@
         <v>0.85</v>
       </c>
       <c r="G55" s="41">
+        <v>0</v>
+      </c>
+      <c r="H55" s="41">
         <v>0.6</v>
       </c>
-      <c r="H55" s="41">
+      <c r="I55" s="41">
         <v>0.45</v>
       </c>
-      <c r="I55" s="46">
+      <c r="J55" s="46">
         <v>0.75</v>
       </c>
-      <c r="J55" s="19" t="s">
+      <c r="K55" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K55" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L55" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M55" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N55" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N55" s="22">
+      <c r="O55" s="22">
         <v>17</v>
       </c>
-      <c r="O55" s="18">
+      <c r="P55" s="18">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P55" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q55" s="15" t="s">
+      <c r="Q55" s="23">
+        <v>1</v>
+      </c>
+      <c r="R55" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="56" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A56" s="91">
         <v>55</v>
       </c>
@@ -9743,41 +9917,44 @@
         <v>1.25</v>
       </c>
       <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
         <v>0.6</v>
       </c>
-      <c r="H56" s="2">
+      <c r="I56" s="2">
         <v>0.75</v>
       </c>
-      <c r="I56" s="46">
+      <c r="J56" s="46">
         <v>0.3</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="K56" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K56" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L56" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M56" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N56" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N56" s="22">
+      <c r="O56" s="22">
         <v>37</v>
       </c>
-      <c r="O56" s="18">
+      <c r="P56" s="18">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P56" s="23">
+      <c r="Q56" s="23">
         <v>2</v>
       </c>
-      <c r="Q56" s="15" t="s">
+      <c r="R56" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="57" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A57" s="91">
         <v>56</v>
       </c>
@@ -9797,42 +9974,45 @@
         <v>1.5</v>
       </c>
       <c r="G57" s="42">
+        <v>0</v>
+      </c>
+      <c r="H57" s="42">
         <v>0.6</v>
       </c>
-      <c r="H57" s="42">
+      <c r="I57" s="42">
         <v>0.95</v>
       </c>
-      <c r="I57" s="46">
+      <c r="J57" s="46">
         <v>0</v>
       </c>
-      <c r="J57" s="29" t="s">
+      <c r="K57" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="K57" s="29" t="s">
-        <v>218</v>
       </c>
       <c r="L57" s="29" t="s">
         <v>218</v>
       </c>
       <c r="M57" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="N57" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="N57" s="24">
+      <c r="O57" s="24">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O57" s="25">
+      <c r="P57" s="25">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P57" s="26">
+      <c r="Q57" s="26">
         <v>4</v>
       </c>
-      <c r="Q57" s="15" t="s">
+      <c r="R57" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="58" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A58" s="91">
         <v>57</v>
       </c>
@@ -9852,41 +10032,44 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
         <v>0.73</v>
       </c>
-      <c r="H58" s="1">
+      <c r="I58" s="1">
         <v>0.1</v>
       </c>
-      <c r="I58" s="45">
+      <c r="J58" s="45">
         <v>0.95</v>
       </c>
-      <c r="J58" s="19" t="s">
+      <c r="K58" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K58" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L58" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M58" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N58" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N58" s="22">
+      <c r="O58" s="22">
         <v>5</v>
       </c>
-      <c r="O58" s="18">
+      <c r="P58" s="18">
         <f t="shared" si="2"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="P58" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q58" s="15" t="s">
+      <c r="Q58" s="21">
+        <v>1</v>
+      </c>
+      <c r="R58" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="59" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A59" s="91">
         <v>58</v>
       </c>
@@ -9906,41 +10089,44 @@
         <v>0.72</v>
       </c>
       <c r="G59" s="2">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2">
         <v>0.73</v>
       </c>
-      <c r="H59" s="2">
+      <c r="I59" s="2">
         <v>0.4</v>
       </c>
-      <c r="I59" s="46">
+      <c r="J59" s="46">
         <v>0.75</v>
       </c>
-      <c r="J59" s="19" t="s">
+      <c r="K59" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K59" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L59" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M59" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N59" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N59" s="22">
+      <c r="O59" s="22">
         <v>20</v>
       </c>
-      <c r="O59" s="18">
+      <c r="P59" s="18">
         <f t="shared" si="2"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="P59" s="23">
+      <c r="Q59" s="23">
         <v>2</v>
       </c>
-      <c r="Q59" s="15" t="s">
+      <c r="R59" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="60" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A60" s="91">
         <v>59</v>
       </c>
@@ -9960,41 +10146,44 @@
         <v>1.66</v>
       </c>
       <c r="G60" s="2">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2">
         <v>0.73</v>
       </c>
-      <c r="H60" s="2">
+      <c r="I60" s="2">
         <v>0.8</v>
       </c>
-      <c r="I60" s="46">
+      <c r="J60" s="46">
         <v>0.3</v>
       </c>
-      <c r="J60" s="19" t="s">
+      <c r="K60" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K60" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L60" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M60" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N60" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N60" s="22">
+      <c r="O60" s="22">
         <v>50</v>
       </c>
-      <c r="O60" s="18">
+      <c r="P60" s="18">
         <f t="shared" si="2"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="P60" s="23">
+      <c r="Q60" s="23">
         <v>4</v>
       </c>
-      <c r="Q60" s="15" t="s">
+      <c r="R60" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="61" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A61" s="91">
         <v>60</v>
       </c>
@@ -10014,42 +10203,45 @@
         <v>2.17</v>
       </c>
       <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
         <v>0.73</v>
       </c>
-      <c r="H61" s="3">
-        <v>1</v>
-      </c>
-      <c r="I61" s="46">
+      <c r="I61" s="3">
+        <v>1</v>
+      </c>
+      <c r="J61" s="46">
         <v>0</v>
       </c>
-      <c r="J61" s="29" t="s">
+      <c r="K61" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="K61" s="29" t="s">
-        <v>218</v>
       </c>
       <c r="L61" s="29" t="s">
         <v>218</v>
       </c>
       <c r="M61" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="N61" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="N61" s="24">
+      <c r="O61" s="24">
         <f>24*30/7</f>
         <v>102.85714285714286</v>
       </c>
-      <c r="O61" s="25">
+      <c r="P61" s="25">
         <f t="shared" si="2"/>
         <v>4.8636546552941553</v>
       </c>
-      <c r="P61" s="26">
+      <c r="Q61" s="26">
         <v>8</v>
       </c>
-      <c r="Q61" s="15" t="s">
+      <c r="R61" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="62" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A62" s="91">
         <v>61</v>
       </c>
@@ -10069,40 +10261,43 @@
         <v>0.15</v>
       </c>
       <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
         <v>0.75</v>
       </c>
-      <c r="H62" s="44">
+      <c r="I62" s="44">
         <v>0.2</v>
       </c>
-      <c r="I62" s="45">
+      <c r="J62" s="45">
         <v>0.95</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="K62" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K62" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L62" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M62" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N62" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N62" s="20">
+      <c r="O62" s="20">
         <v>5</v>
       </c>
-      <c r="O62" s="10">
+      <c r="P62" s="10">
         <v>0.30397841595588471</v>
       </c>
-      <c r="P62" s="21">
+      <c r="Q62" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q62" s="15" t="s">
+      <c r="R62" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="63" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A63" s="91">
         <v>62</v>
       </c>
@@ -10122,40 +10317,43 @@
         <v>0.36</v>
       </c>
       <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
         <v>0.65</v>
       </c>
-      <c r="H63" s="41">
+      <c r="I63" s="41">
         <v>0.45</v>
       </c>
-      <c r="I63" s="46">
+      <c r="J63" s="46">
         <v>0.75</v>
       </c>
-      <c r="J63" s="19" t="s">
+      <c r="K63" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K63" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L63" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M63" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N63" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N63" s="22">
+      <c r="O63" s="22">
         <v>17</v>
       </c>
-      <c r="O63" s="18">
+      <c r="P63" s="18">
         <v>0.60795683191176941</v>
       </c>
-      <c r="P63" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q63" s="15" t="s">
+      <c r="Q63" s="23">
+        <v>1</v>
+      </c>
+      <c r="R63" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="64" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A64" s="91">
         <v>63</v>
       </c>
@@ -10175,40 +10373,43 @@
         <v>0.72</v>
       </c>
       <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
         <v>0.65</v>
       </c>
-      <c r="H64" s="41">
+      <c r="I64" s="41">
         <v>0.75</v>
       </c>
-      <c r="I64" s="46">
+      <c r="J64" s="46">
         <v>0.3</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="K64" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K64" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L64" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M64" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N64" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N64" s="22">
+      <c r="O64" s="22">
         <v>37</v>
       </c>
-      <c r="O64" s="18">
+      <c r="P64" s="18">
         <v>1.2159136638235388</v>
       </c>
-      <c r="P64" s="23">
+      <c r="Q64" s="23">
         <v>2</v>
       </c>
-      <c r="Q64" s="15" t="s">
+      <c r="R64" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="65" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A65" s="91">
         <v>64</v>
       </c>
@@ -10228,41 +10429,44 @@
         <v>1.5</v>
       </c>
       <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
         <v>0.8</v>
       </c>
-      <c r="H65" s="42">
+      <c r="I65" s="42">
         <v>0.95</v>
       </c>
-      <c r="I65" s="47">
+      <c r="J65" s="47">
         <v>0</v>
       </c>
-      <c r="J65" s="29" t="s">
+      <c r="K65" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="K65" s="29" t="s">
-        <v>218</v>
       </c>
       <c r="L65" s="29" t="s">
         <v>218</v>
       </c>
       <c r="M65" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="N65" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="N65" s="24">
+      <c r="O65" s="24">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O65" s="29">
+      <c r="P65" s="29">
         <v>2.4318273276470777</v>
       </c>
-      <c r="P65" s="26">
+      <c r="Q65" s="26">
         <v>4</v>
       </c>
-      <c r="Q65" s="15" t="s">
+      <c r="R65" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="66" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A66" s="91">
         <v>65</v>
       </c>
@@ -10282,40 +10486,43 @@
         <v>10</v>
       </c>
       <c r="G66" s="1">
-        <v>1</v>
-      </c>
-      <c r="H66" s="44">
         <v>0</v>
       </c>
-      <c r="I66" s="45">
-        <v>1</v>
-      </c>
-      <c r="J66" s="19" t="s">
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+      <c r="I66" s="44">
+        <v>0</v>
+      </c>
+      <c r="J66" s="45">
+        <v>1</v>
+      </c>
+      <c r="K66" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K66" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L66" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M66" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N66" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N66" s="20">
+      <c r="O66" s="20">
         <v>5</v>
       </c>
-      <c r="O66" s="10">
+      <c r="P66" s="10">
         <v>0.30397841595588471</v>
       </c>
-      <c r="P66" s="21">
+      <c r="Q66" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q66" s="15" t="s">
+      <c r="R66" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="67" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A67" s="91">
         <v>66</v>
       </c>
@@ -10335,40 +10542,43 @@
         <v>10</v>
       </c>
       <c r="G67" s="2">
-        <v>1</v>
-      </c>
-      <c r="H67" s="41">
         <v>0</v>
       </c>
-      <c r="I67" s="46">
-        <v>1</v>
-      </c>
-      <c r="J67" s="19" t="s">
+      <c r="H67" s="2">
+        <v>1</v>
+      </c>
+      <c r="I67" s="41">
+        <v>0</v>
+      </c>
+      <c r="J67" s="46">
+        <v>1</v>
+      </c>
+      <c r="K67" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K67" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L67" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M67" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N67" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N67" s="22">
+      <c r="O67" s="22">
         <v>17</v>
       </c>
-      <c r="O67" s="18">
+      <c r="P67" s="18">
         <v>0.60795683191176941</v>
       </c>
-      <c r="P67" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="15" t="s">
+      <c r="Q67" s="23">
+        <v>1</v>
+      </c>
+      <c r="R67" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="68" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A68" s="91">
         <v>67</v>
       </c>
@@ -10388,40 +10598,43 @@
         <v>10</v>
       </c>
       <c r="G68" s="2">
-        <v>1</v>
-      </c>
-      <c r="H68" s="41">
         <v>0</v>
       </c>
-      <c r="I68" s="46">
-        <v>1</v>
-      </c>
-      <c r="J68" s="19" t="s">
+      <c r="H68" s="2">
+        <v>1</v>
+      </c>
+      <c r="I68" s="41">
+        <v>0</v>
+      </c>
+      <c r="J68" s="46">
+        <v>1</v>
+      </c>
+      <c r="K68" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="K68" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="L68" s="19" t="s">
         <v>218</v>
       </c>
       <c r="M68" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N68" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="N68" s="22">
+      <c r="O68" s="22">
         <v>37</v>
       </c>
-      <c r="O68" s="18">
+      <c r="P68" s="18">
         <v>1.2159136638235388</v>
       </c>
-      <c r="P68" s="23">
+      <c r="Q68" s="23">
         <v>2</v>
       </c>
-      <c r="Q68" s="15" t="s">
+      <c r="R68" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="69" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1">
+    <row r="69" spans="1:18" s="16" customFormat="1" ht="14" customHeight="1">
       <c r="A69" s="91">
         <v>68</v>
       </c>
@@ -10441,161 +10654,164 @@
         <v>10</v>
       </c>
       <c r="G69" s="3">
-        <v>1</v>
-      </c>
-      <c r="H69" s="42">
         <v>0</v>
       </c>
-      <c r="I69" s="47">
-        <v>1</v>
-      </c>
-      <c r="J69" s="29" t="s">
+      <c r="H69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="42">
+        <v>0</v>
+      </c>
+      <c r="J69" s="47">
+        <v>1</v>
+      </c>
+      <c r="K69" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="K69" s="29" t="s">
-        <v>218</v>
       </c>
       <c r="L69" s="29" t="s">
         <v>218</v>
       </c>
       <c r="M69" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="N69" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="N69" s="24">
+      <c r="O69" s="24">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="O69" s="29">
+      <c r="P69" s="29">
         <v>2.4318273276470777</v>
       </c>
-      <c r="P69" s="26">
+      <c r="Q69" s="26">
         <v>4</v>
       </c>
-      <c r="Q69" s="15" t="s">
+      <c r="R69" s="15" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B5:Q68">
+  <sortState ref="B5:R68">
     <sortCondition ref="B133:B196"/>
     <sortCondition ref="C133:C196"/>
   </sortState>
-  <conditionalFormatting sqref="F10:H13">
+  <conditionalFormatting sqref="F10:I13">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:H9">
+  <conditionalFormatting sqref="F2:I9">
     <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:H17">
+  <conditionalFormatting sqref="F14:I17">
     <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:G25">
+  <conditionalFormatting sqref="F22:H25">
     <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:H29">
+  <conditionalFormatting sqref="F26:I29">
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42:H45">
+  <conditionalFormatting sqref="F42:I45">
     <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:G41">
+  <conditionalFormatting sqref="F38:H41">
     <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:G21">
+  <conditionalFormatting sqref="F18:H21">
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F54:G57">
+  <conditionalFormatting sqref="F54:H57">
     <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F50:H53">
+  <conditionalFormatting sqref="F50:I53">
     <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58:G61">
+  <conditionalFormatting sqref="F58:H61">
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58:H61">
+  <conditionalFormatting sqref="I58:I61">
     <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F46:G49">
+  <conditionalFormatting sqref="F46:H49">
     <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H21">
+  <conditionalFormatting sqref="I18:I21">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H25">
+  <conditionalFormatting sqref="I22:I25">
     <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:H41">
+  <conditionalFormatting sqref="I38:I41">
     <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46:H49">
+  <conditionalFormatting sqref="I46:I49">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54:H57">
+  <conditionalFormatting sqref="I54:I57">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62:G65">
+  <conditionalFormatting sqref="F62:H65">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62:H65">
+  <conditionalFormatting sqref="I62:I65">
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66:G69">
+  <conditionalFormatting sqref="F66:H69">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H66:H69">
+  <conditionalFormatting sqref="I66:I69">
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",H66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",I66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:H33">
+  <conditionalFormatting sqref="F30:I33">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:H37">
+  <conditionalFormatting sqref="F34:I37">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",F34)))</formula>
     </cfRule>

</xml_diff>